<commit_message>
commit here on 29 aug 2017
</commit_message>
<xml_diff>
--- a/test-Data/testDatFile.xlsx
+++ b/test-Data/testDatFile.xlsx
@@ -4,35 +4,36 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="14280" windowHeight="3480"/>
   </bookViews>
   <sheets>
     <sheet name="LoginData" sheetId="1" r:id="rId1"/>
     <sheet name="URL" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="122211"/>
+  <calcPr calcId="0"/>
+  <oleSize ref="A1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
   <si>
+    <t>UserName</t>
+  </si>
+  <si>
+    <t>Password</t>
+  </si>
+  <si>
+    <t>URL</t>
+  </si>
+  <si>
+    <t>https://wordpress.com/log-in</t>
+  </si>
+  <si>
     <t>sreejith47</t>
   </si>
   <si>
     <t>*Sree1986</t>
-  </si>
-  <si>
-    <t>UserName</t>
-  </si>
-  <si>
-    <t>Password</t>
-  </si>
-  <si>
-    <t>URL</t>
-  </si>
-  <si>
-    <t>https://wordpress.com/log-in</t>
   </si>
 </sst>
 </file>
@@ -387,8 +388,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -399,18 +400,18 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B1" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -422,7 +423,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B1"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
@@ -433,10 +434,10 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>